<commit_message>
EPBDS-6429 Add tests for Boolean[] type
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test/rules/functionality/Boolean.xlsx
+++ b/DEV/org.openl.test/test/rules/functionality/Boolean.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="primitive" sheetId="1" r:id="rId1"/>
+    <sheet name="Object" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="40">
   <si>
     <t>Result</t>
   </si>
@@ -128,6 +129,12 @@
   </si>
   <si>
     <t>_res_.$xor$res</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult Booleans (Boolean[] values)</t>
+  </si>
+  <si>
+    <t>Test Booleans BooleansTest</t>
   </si>
 </sst>
 </file>
@@ -527,14 +534,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -965,4 +976,451 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>